<commit_message>
fitur jika ada score yang sama
</commit_message>
<xml_diff>
--- a/peringkat.xlsx
+++ b/peringkat.xlsx
@@ -457,10 +457,10 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>79</v>
+        <v>24</v>
       </c>
       <c r="B2" t="n">
-        <v>87</v>
+        <v>100</v>
       </c>
       <c r="C2" t="n">
         <v>9</v>
@@ -471,10 +471,10 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>69</v>
+        <v>42</v>
       </c>
       <c r="B3" t="n">
-        <v>86</v>
+        <v>94</v>
       </c>
       <c r="C3" t="n">
         <v>10</v>
@@ -485,13 +485,13 @@
     </row>
     <row r="4">
       <c r="A4" t="n">
-        <v>42</v>
+        <v>79</v>
       </c>
       <c r="B4" t="n">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C4" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" t="n">
         <v>83.33333333333333</v>
@@ -499,13 +499,13 @@
     </row>
     <row r="5">
       <c r="A5" t="n">
-        <v>24</v>
+        <v>69</v>
       </c>
       <c r="B5" t="n">
-        <v>100</v>
+        <v>86</v>
       </c>
       <c r="C5" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="D5" t="n">
         <v>83.33333333333333</v>
@@ -583,16 +583,16 @@
     </row>
     <row r="11">
       <c r="A11" t="n">
-        <v>16</v>
+        <v>54</v>
       </c>
       <c r="B11" t="n">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="C11" t="n">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="D11" t="n">
-        <v>75.57692307692308</v>
+        <v>76.02689486552569</v>
       </c>
     </row>
   </sheetData>

</xml_diff>